<commit_message>
feat: enhance batch import functionality with layer matching and skipped entries notification
</commit_message>
<xml_diff>
--- a/Template Preenchido Upper Skin Grid_RevB.xlsx
+++ b/Template Preenchido Upper Skin Grid_RevB.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pribe\OneDrive\Documents\GitHub\GridLamEdit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7522E065-C389-4A4F-AC70-A2B68EE5F019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D587F1-174C-45EF-BF19-70CAB293E0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Geral" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -385,7 +385,7 @@
   <dimension ref="A1:BQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +442,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>

</xml_diff>